<commit_message>
fix: 0.20.56-beta kleine naamgeving en bug fix
</commit_message>
<xml_diff>
--- a/db/PedMedCont.xlsx
+++ b/db/PedMedCont.xlsx
@@ -722,7 +722,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,13 +1444,13 @@
         <v>50</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I16">
         <v>50</v>
       </c>
       <c r="J16">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="K16">
         <v>50</v>
@@ -1465,7 +1465,7 @@
         <v>10</v>
       </c>
       <c r="P16">
-        <v>10</v>
+        <v>0.05</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1818,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="P23">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="Q23">
         <v>0</v>

</xml_diff>

<commit_message>
feat: v0.50.22-beta added eGFR, and ped med cont features
</commit_message>
<xml_diff>
--- a/db/PedMedCont.xlsx
+++ b/db/PedMedCont.xlsx
@@ -16,14 +16,14 @@
   </externalReferences>
   <definedNames>
     <definedName name="_Pat_Gewicht">[1]PatDetails!$B$6</definedName>
-    <definedName name="Tbl_Admin_PedMedCont" localSheetId="0">Tbl_Admin_PedMedCont!$A$4:$R$34</definedName>
+    <definedName name="Tbl_Admin_PedMedCont" localSheetId="0">Tbl_Admin_PedMedCont!$A$4:$R$35</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t>adrenaline</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>NaCl 3%</t>
+  </si>
+  <si>
+    <t>nicardipine</t>
   </si>
 </sst>
 </file>
@@ -294,6 +297,7 @@
       <sheetName val="Global--&gt;"/>
       <sheetName val="GlobGuiFront"/>
       <sheetName val="GlobGuiMedDisc"/>
+      <sheetName val="GlobPrtMedDisc"/>
       <sheetName val="GlobBerMedDisc"/>
       <sheetName val="GlobTblMedDisc"/>
       <sheetName val="GlobTblMedOpdr"/>
@@ -375,14 +379,14 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
-      <sheetData sheetId="18">
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19">
         <row r="6">
           <cell r="B6">
             <v>0</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
@@ -427,6 +431,7 @@
       <sheetData sheetId="61"/>
       <sheetData sheetId="62"/>
       <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -720,10 +725,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2029,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -2033,25 +2038,25 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>50</v>
       </c>
       <c r="F28">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <v>50</v>
       </c>
       <c r="H28">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I28">
         <v>50</v>
       </c>
       <c r="J28">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="K28">
         <v>50</v>
@@ -2060,13 +2065,13 @@
         <v>0.5</v>
       </c>
       <c r="M28">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N28">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P28">
-        <v>10</v>
+        <v>0.2</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -2074,7 +2079,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -2083,40 +2088,40 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E29">
         <v>50</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G29">
         <v>50</v>
       </c>
       <c r="H29">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I29">
         <v>50</v>
       </c>
       <c r="J29">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="K29">
         <v>50</v>
       </c>
       <c r="L29">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="M29">
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -2124,54 +2129,57 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="H30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="J30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="L30">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="M30">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="N30">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -2180,25 +2188,25 @@
         <v>18</v>
       </c>
       <c r="D31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I31">
         <v>1</v>
       </c>
       <c r="J31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -2218,7 +2226,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -2227,93 +2235,87 @@
         <v>18</v>
       </c>
       <c r="D32">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E32">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="G32">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="H32">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="I32">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="J32">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="K32">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="L32">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="M32">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="N32">
-        <v>2</v>
-      </c>
-      <c r="P32">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="Q32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E33">
         <v>50</v>
       </c>
       <c r="F33">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G33">
         <v>50</v>
       </c>
       <c r="H33">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="I33">
         <v>50</v>
       </c>
       <c r="J33">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="K33">
         <v>50</v>
       </c>
       <c r="L33">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="M33">
-        <v>10</v>
+        <v>1.2</v>
       </c>
       <c r="N33">
-        <v>15</v>
-      </c>
-      <c r="O33">
-        <v>5.0000000000000001E-3</v>
+        <v>2</v>
       </c>
       <c r="P33">
-        <v>0.42</v>
+        <v>10</v>
       </c>
       <c r="Q33">
         <v>0</v>
@@ -2321,57 +2323,110 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>50</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <v>50</v>
+      </c>
+      <c r="H34">
+        <v>20</v>
+      </c>
+      <c r="I34">
+        <v>50</v>
+      </c>
+      <c r="J34">
+        <v>20</v>
+      </c>
+      <c r="K34">
+        <v>50</v>
+      </c>
+      <c r="L34">
+        <v>0.1</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+      <c r="N34">
+        <v>15</v>
+      </c>
+      <c r="O34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P34">
+        <v>0.42</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>43</v>
       </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
         <v>18</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>1250</v>
       </c>
-      <c r="E34">
-        <v>50</v>
-      </c>
-      <c r="F34">
+      <c r="E35">
+        <v>50</v>
+      </c>
+      <c r="F35">
         <v>1250</v>
       </c>
-      <c r="G34">
-        <v>50</v>
-      </c>
-      <c r="H34">
+      <c r="G35">
+        <v>50</v>
+      </c>
+      <c r="H35">
         <v>1250</v>
       </c>
-      <c r="I34">
-        <v>50</v>
-      </c>
-      <c r="J34">
+      <c r="I35">
+        <v>50</v>
+      </c>
+      <c r="J35">
         <v>1250</v>
       </c>
-      <c r="K34">
-        <v>50</v>
-      </c>
-      <c r="L34">
+      <c r="K35">
+        <v>50</v>
+      </c>
+      <c r="L35">
         <v>5</v>
       </c>
-      <c r="M34">
-        <v>10</v>
-      </c>
-      <c r="N34">
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35">
         <v>20</v>
       </c>
-      <c r="O34">
+      <c r="O35">
         <v>5</v>
       </c>
-      <c r="P34">
+      <c r="P35">
         <v>25</v>
       </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34" t="s">
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>